<commit_message>
Updated author pages to have '.' in the degree abbreviations
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Brian_Kielstra/BKielstra_Author_form.xlsx
+++ b/website_content_creation/authors/Brian_Kielstra/BKielstra_Author_form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\Documents\WET lab\WETlab_website\website_content_creation\Brian_Kielstra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\Documents\WET lab\WETlab_website\website_content_creation\authors\Brian_Kielstra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -110,21 +110,12 @@
     <t>https://scholar.google.ca/citations?hl=en&amp;inst=17001591832933267808&amp;user=qaB6gp8AAAAJ</t>
   </si>
   <si>
-    <t>PhD Forestry</t>
-  </si>
-  <si>
-    <t>MSc Biology</t>
-  </si>
-  <si>
     <t>Queen's University (Arnott and Gunn)</t>
   </si>
   <si>
     <t>University of British Columbia (Richardson)</t>
   </si>
   <si>
-    <t>BSc Environmental Science</t>
-  </si>
-  <si>
     <t>University of Guelph (Natural Resources Management Co-op)</t>
   </si>
   <si>
@@ -144,6 +135,15 @@
   </si>
   <si>
     <t>Watershed Ecology Team</t>
+  </si>
+  <si>
+    <t>Ph.D. Forestry</t>
+  </si>
+  <si>
+    <t>M.Sc. Biology</t>
+  </si>
+  <si>
+    <t>B.Sc. Environmental Science</t>
   </si>
 </sst>
 </file>
@@ -401,6 +401,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,8 +412,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -696,7 +696,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -773,7 +773,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -783,11 +783,11 @@
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>39</v>
+      <c r="A12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -796,11 +796,11 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
@@ -815,10 +815,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2">
         <v>2020</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1">
         <v>2014</v>
@@ -837,10 +837,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1">
         <v>2010</v>
@@ -858,10 +858,10 @@
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="18"/>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
@@ -910,17 +910,17 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated to include Alexandra Clark Profile
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Brian_Kielstra/BKielstra_Author_form.xlsx
+++ b/website_content_creation/authors/Brian_Kielstra/BKielstra_Author_form.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmender\RProjects\GLFC-WET.github.io\website_content_creation\authors\Brian_Kielstra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Brian_Kielstra/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0A549B3ACB4AC6ABE16F1E5D71486CDF326C314B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{661908BD-9B77-4C73-A6F2-5265E003D086}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,9 +132,6 @@
     <t>Groups</t>
   </si>
   <si>
-    <t>Watershed Ecology Team</t>
-  </si>
-  <si>
     <t>Ph.D. Forestry</t>
   </si>
   <si>
@@ -150,12 +148,15 @@
   </si>
   <si>
     <t>brian.kielstra@NRCan-RNCan.gc.ca</t>
+  </si>
+  <si>
+    <t>Past WETlab Members</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -706,31 +707,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
-    <col min="2" max="2" width="56.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -738,7 +739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
@@ -746,21 +747,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
@@ -768,13 +769,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -782,15 +783,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -798,33 +799,33 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
     </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -835,9 +836,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
@@ -846,9 +847,9 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>27</v>
@@ -857,9 +858,9 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
@@ -868,24 +869,24 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="19"/>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>10</v>
       </c>
@@ -893,7 +894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>12</v>
       </c>
@@ -901,56 +902,56 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
   </sheetData>
@@ -959,9 +960,9 @@
     <mergeCell ref="A23:B23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B25" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B25" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>